<commit_message>
Tied Registry into parser
</commit_message>
<xml_diff>
--- a/module/Import/test/ImportTest/Importer/Nyc/Parser/Excel/_files/class_invalid_ddbnnn.xlsx
+++ b/module/Import/test/ImportTest/Importer/Nyc/Parser/Excel/_files/class_invalid_ddbnnn.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="33520" windowHeight="20540"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000"/>
   </bookViews>
   <sheets>
     <sheet name="Classes" sheetId="1" r:id="rId1"/>
@@ -413,7 +413,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A2" sqref="A2:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>